<commit_message>
feat: Add name for checked or approved at export IPA
</commit_message>
<xml_diff>
--- a/public/assets/file/Template IPA.xlsx
+++ b/public/assets/file/Template IPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EAEF4B-47C5-4B2C-ABDE-13E7AEA7DAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B19E8A-763D-4522-9E3B-1136A463BB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,7 +269,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -429,15 +429,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -453,19 +444,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -525,17 +503,6 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -768,11 +735,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -862,9 +954,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -890,10 +979,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -933,16 +1019,58 @@
     <xf numFmtId="9" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -950,6 +1078,46 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -963,109 +1131,53 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,13 +1437,13 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.453125" style="48" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" style="47" customWidth="1"/>
     <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="3" width="14.453125" customWidth="1"/>
     <col min="4" max="4" width="17.90625" customWidth="1"/>
@@ -1349,7 +1461,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45"/>
+      <c r="A1" s="44"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1381,20 +1493,20 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -1415,20 +1527,20 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -1449,7 +1561,7 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1481,7 +1593,7 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1509,7 +1621,7 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="21"/>
@@ -1545,10 +1657,10 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="74"/>
+      <c r="B7" s="106"/>
       <c r="C7" s="26" t="s">
         <v>7</v>
       </c>
@@ -1581,7 +1693,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="30"/>
@@ -1617,7 +1729,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1645,7 +1757,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="34"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1675,41 +1787,41 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="78" t="s">
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="79"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="70" t="s">
+      <c r="G11" s="111"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="70" t="s">
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="71"/>
-      <c r="O11" s="71"/>
-      <c r="P11" s="71"/>
-      <c r="Q11" s="72"/>
-      <c r="R11" s="78" t="s">
+      <c r="N11" s="85"/>
+      <c r="O11" s="85"/>
+      <c r="P11" s="85"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="80"/>
-      <c r="T11" s="43" t="s">
+      <c r="S11" s="94"/>
+      <c r="T11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="U11" s="44"/>
+      <c r="U11" s="43"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -1717,33 +1829,33 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="105" t="s">
+      <c r="A12" s="110"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="106"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="102"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="104"/>
-      <c r="M12" s="102"/>
-      <c r="N12" s="103"/>
-      <c r="O12" s="103"/>
-      <c r="P12" s="103"/>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="105" t="s">
+      <c r="G12" s="112"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="S12" s="107"/>
-      <c r="T12" s="105" t="s">
+      <c r="S12" s="92"/>
+      <c r="T12" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="U12" s="108"/>
+      <c r="U12" s="91"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -1751,27 +1863,27 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="99"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="100"/>
-      <c r="T13" s="53"/>
-      <c r="U13" s="93"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="51"/>
+      <c r="S13" s="83"/>
+      <c r="T13" s="51"/>
+      <c r="U13" s="76"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -1779,27 +1891,27 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="97"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="85"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="58"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="95"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="69"/>
+      <c r="R14" s="56"/>
+      <c r="S14" s="69"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="78"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -1807,40 +1919,40 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="86"/>
-      <c r="B15" s="109" t="s">
+      <c r="A15" s="70"/>
+      <c r="B15" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="112">
+      <c r="C15" s="96"/>
+      <c r="D15" s="96"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98">
         <f ca="1">SUM(F13:H59)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="110"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="114"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="115" t="s">
+      <c r="G15" s="96"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="110"/>
-      <c r="O15" s="110"/>
-      <c r="P15" s="110"/>
-      <c r="Q15" s="111"/>
-      <c r="R15" s="116">
+      <c r="N15" s="96"/>
+      <c r="O15" s="96"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="97"/>
+      <c r="R15" s="101">
         <f ca="1">SUM(R13:S59)</f>
         <v>0</v>
       </c>
-      <c r="S15" s="113"/>
-      <c r="T15" s="117">
+      <c r="S15" s="99"/>
+      <c r="T15" s="102">
         <f ca="1">SUM(T13:U59)</f>
         <v>0</v>
       </c>
-      <c r="U15" s="118"/>
+      <c r="U15" s="103"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -1848,7 +1960,7 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
@@ -1856,25 +1968,25 @@
       <c r="F16" s="38"/>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="83"/>
-      <c r="K16" s="83"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="52" t="s">
+      <c r="J16" s="114"/>
+      <c r="K16" s="123"/>
+      <c r="L16" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="N16" s="83"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="84"/>
-      <c r="Q16" s="52" t="s">
+      <c r="M16" s="117"/>
+      <c r="N16" s="117"/>
+      <c r="O16" s="117"/>
+      <c r="P16" s="118"/>
+      <c r="Q16" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="83"/>
-      <c r="S16" s="83"/>
-      <c r="T16" s="83"/>
-      <c r="U16" s="91"/>
+      <c r="R16" s="114"/>
+      <c r="S16" s="114"/>
+      <c r="T16" s="114"/>
+      <c r="U16" s="115"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -1882,27 +1994,27 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="88"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="39"/>
       <c r="J17" s="23"/>
       <c r="K17" s="23"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
       <c r="Q17" s="39"/>
       <c r="R17" s="23"/>
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
-      <c r="U17" s="92"/>
+      <c r="U17" s="75"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -1910,27 +2022,27 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="40"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="121"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
       <c r="Q18" s="40"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="93"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="76"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
@@ -1938,27 +2050,27 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
       <c r="I19" s="40"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="121"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
       <c r="Q19" s="40"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="93"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="76"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
@@ -1966,27 +2078,27 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
       <c r="I20" s="40"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="121"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
       <c r="Q20" s="40"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="53"/>
-      <c r="T20" s="53"/>
-      <c r="U20" s="93"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="76"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
@@ -1994,27 +2106,27 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="88"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
       <c r="I21" s="40"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="121"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
       <c r="Q21" s="40"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="53"/>
-      <c r="T21" s="53"/>
-      <c r="U21" s="93"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="76"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
@@ -2022,27 +2134,27 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="88"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="81"/>
-      <c r="S22" s="81"/>
-      <c r="T22" s="81"/>
-      <c r="U22" s="94"/>
+      <c r="A22" s="72"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="122"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="68"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
+      <c r="T22" s="67"/>
+      <c r="U22" s="77"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
@@ -2050,33 +2162,33 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="89"/>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="67" t="s">
+      <c r="A23" s="73"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="66" t="s">
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="N23" s="66"/>
-      <c r="O23" s="66"/>
-      <c r="P23" s="66"/>
-      <c r="Q23" s="67" t="s">
+      <c r="M23" s="126"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="R23" s="66"/>
-      <c r="S23" s="66"/>
-      <c r="T23" s="66"/>
-      <c r="U23" s="69"/>
+      <c r="R23" s="64"/>
+      <c r="S23" s="64"/>
+      <c r="T23" s="64"/>
+      <c r="U23" s="66"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
@@ -2084,27 +2196,27 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="90"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="53"/>
-      <c r="U24" s="53"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="125"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="51"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -2112,27 +2224,27 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
-      <c r="P25" s="53"/>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="53"/>
-      <c r="S25" s="53"/>
-      <c r="T25" s="53"/>
-      <c r="U25" s="53"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="51"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -2140,27 +2252,27 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="53"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="53"/>
-      <c r="T26" s="53"/>
-      <c r="U26" s="53"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
@@ -2168,27 +2280,27 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="51"/>
+      <c r="S27" s="51"/>
+      <c r="T27" s="51"/>
+      <c r="U27" s="51"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
@@ -2196,27 +2308,27 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="53"/>
-      <c r="S28" s="53"/>
-      <c r="T28" s="53"/>
-      <c r="U28" s="53"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="51"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
@@ -2224,27 +2336,27 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="53"/>
-      <c r="P29" s="53"/>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="53"/>
-      <c r="T29" s="53"/>
-      <c r="U29" s="53"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="51"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
@@ -2252,27 +2364,27 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="53"/>
-      <c r="O30" s="53"/>
-      <c r="P30" s="53"/>
-      <c r="Q30" s="53"/>
-      <c r="R30" s="53"/>
-      <c r="S30" s="53"/>
-      <c r="T30" s="53"/>
-      <c r="U30" s="53"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="51"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
@@ -2280,27 +2392,27 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="59"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="53"/>
-      <c r="P31" s="53"/>
-      <c r="Q31" s="53"/>
-      <c r="R31" s="53"/>
-      <c r="S31" s="53"/>
-      <c r="T31" s="53"/>
-      <c r="U31" s="53"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="51"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
@@ -2308,27 +2420,27 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="59"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="53"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="53"/>
-      <c r="R32" s="53"/>
-      <c r="S32" s="53"/>
-      <c r="T32" s="53"/>
-      <c r="U32" s="53"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="51"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="57"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="51"/>
+      <c r="P32" s="51"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="51"/>
+      <c r="S32" s="51"/>
+      <c r="T32" s="51"/>
+      <c r="U32" s="51"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
@@ -2336,27 +2448,27 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="53"/>
-      <c r="S33" s="53"/>
-      <c r="T33" s="53"/>
-      <c r="U33" s="53"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="51"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
@@ -2364,27 +2476,27 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="59"/>
-      <c r="N34" s="53"/>
-      <c r="O34" s="53"/>
-      <c r="P34" s="53"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="53"/>
-      <c r="S34" s="53"/>
-      <c r="T34" s="53"/>
-      <c r="U34" s="53"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="57"/>
+      <c r="N34" s="51"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="51"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="51"/>
+      <c r="T34" s="51"/>
+      <c r="U34" s="51"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
@@ -2392,27 +2504,27 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="59"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53"/>
-      <c r="P35" s="53"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="53"/>
-      <c r="S35" s="53"/>
-      <c r="T35" s="53"/>
-      <c r="U35" s="53"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="51"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
@@ -2420,27 +2532,27 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="53"/>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
-      <c r="T36" s="53"/>
-      <c r="U36" s="53"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="51"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
@@ -2448,27 +2560,27 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="53"/>
-      <c r="O37" s="53"/>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="53"/>
-      <c r="R37" s="53"/>
-      <c r="S37" s="53"/>
-      <c r="T37" s="53"/>
-      <c r="U37" s="53"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="51"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
@@ -2476,27 +2588,27 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="53"/>
-      <c r="O38" s="53"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="53"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="53"/>
-      <c r="T38" s="53"/>
-      <c r="U38" s="53"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="51"/>
+      <c r="T38" s="51"/>
+      <c r="U38" s="51"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
@@ -2504,27 +2616,27 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="60"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="53"/>
-      <c r="S39" s="53"/>
-      <c r="T39" s="53"/>
-      <c r="U39" s="53"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="51"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
@@ -2532,27 +2644,27 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
-      <c r="O40" s="53"/>
-      <c r="P40" s="53"/>
-      <c r="Q40" s="53"/>
-      <c r="R40" s="53"/>
-      <c r="S40" s="53"/>
-      <c r="T40" s="53"/>
-      <c r="U40" s="53"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="56"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="51"/>
+      <c r="O40" s="51"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="51"/>
+      <c r="R40" s="51"/>
+      <c r="S40" s="51"/>
+      <c r="T40" s="51"/>
+      <c r="U40" s="51"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
@@ -2560,27 +2672,27 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="54"/>
-      <c r="B41" s="55"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="60"/>
-      <c r="N41" s="53"/>
-      <c r="O41" s="53"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="53"/>
-      <c r="R41" s="53"/>
-      <c r="S41" s="53"/>
-      <c r="T41" s="53"/>
-      <c r="U41" s="53"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="58"/>
+      <c r="N41" s="51"/>
+      <c r="O41" s="51"/>
+      <c r="P41" s="51"/>
+      <c r="Q41" s="51"/>
+      <c r="R41" s="51"/>
+      <c r="S41" s="51"/>
+      <c r="T41" s="51"/>
+      <c r="U41" s="51"/>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
@@ -2588,27 +2700,27 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="60"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="53"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="51"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="51"/>
+      <c r="T42" s="51"/>
+      <c r="U42" s="51"/>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
@@ -2616,27 +2728,27 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="54"/>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="60"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="53"/>
-      <c r="O43" s="53"/>
-      <c r="P43" s="53"/>
-      <c r="Q43" s="53"/>
-      <c r="R43" s="53"/>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
-      <c r="U43" s="53"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="51"/>
+      <c r="O43" s="51"/>
+      <c r="P43" s="51"/>
+      <c r="Q43" s="51"/>
+      <c r="R43" s="51"/>
+      <c r="S43" s="51"/>
+      <c r="T43" s="51"/>
+      <c r="U43" s="51"/>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
@@ -2644,27 +2756,27 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="54"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="60"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="60"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="53"/>
-      <c r="P44" s="53"/>
-      <c r="Q44" s="53"/>
-      <c r="R44" s="53"/>
-      <c r="S44" s="53"/>
-      <c r="T44" s="53"/>
-      <c r="U44" s="53"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="51"/>
+      <c r="O44" s="51"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="51"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="51"/>
+      <c r="T44" s="51"/>
+      <c r="U44" s="51"/>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
@@ -2672,27 +2784,27 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="60"/>
-      <c r="N45" s="53"/>
-      <c r="O45" s="53"/>
-      <c r="P45" s="53"/>
-      <c r="Q45" s="53"/>
-      <c r="R45" s="53"/>
-      <c r="S45" s="53"/>
-      <c r="T45" s="53"/>
-      <c r="U45" s="53"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="51"/>
+      <c r="O45" s="51"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="51"/>
+      <c r="R45" s="51"/>
+      <c r="S45" s="51"/>
+      <c r="T45" s="51"/>
+      <c r="U45" s="51"/>
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
@@ -2700,27 +2812,27 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="60"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="53"/>
-      <c r="L46" s="53"/>
-      <c r="M46" s="60"/>
-      <c r="N46" s="53"/>
-      <c r="O46" s="53"/>
-      <c r="P46" s="53"/>
-      <c r="Q46" s="53"/>
-      <c r="R46" s="53"/>
-      <c r="S46" s="53"/>
-      <c r="T46" s="53"/>
-      <c r="U46" s="53"/>
+      <c r="A46" s="52"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="51"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51"/>
+      <c r="R46" s="51"/>
+      <c r="S46" s="51"/>
+      <c r="T46" s="51"/>
+      <c r="U46" s="51"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
@@ -2728,27 +2840,27 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="54"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="53"/>
-      <c r="L47" s="53"/>
-      <c r="M47" s="53"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="53"/>
-      <c r="P47" s="53"/>
-      <c r="Q47" s="53"/>
-      <c r="R47" s="53"/>
-      <c r="S47" s="53"/>
-      <c r="T47" s="53"/>
-      <c r="U47" s="53"/>
+      <c r="A47" s="52"/>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51"/>
+      <c r="R47" s="51"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="51"/>
+      <c r="U47" s="51"/>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
@@ -2756,27 +2868,27 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="60"/>
-      <c r="J48" s="60"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="53"/>
-      <c r="M48" s="59"/>
-      <c r="N48" s="53"/>
-      <c r="O48" s="53"/>
-      <c r="P48" s="53"/>
-      <c r="Q48" s="53"/>
-      <c r="R48" s="53"/>
-      <c r="S48" s="53"/>
-      <c r="T48" s="53"/>
-      <c r="U48" s="53"/>
+      <c r="A48" s="52"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="56"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="57"/>
+      <c r="N48" s="51"/>
+      <c r="O48" s="51"/>
+      <c r="P48" s="51"/>
+      <c r="Q48" s="51"/>
+      <c r="R48" s="51"/>
+      <c r="S48" s="51"/>
+      <c r="T48" s="51"/>
+      <c r="U48" s="51"/>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
@@ -2784,27 +2896,27 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="54"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="60"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="53"/>
-      <c r="M49" s="59"/>
-      <c r="N49" s="53"/>
-      <c r="O49" s="53"/>
-      <c r="P49" s="53"/>
-      <c r="Q49" s="53"/>
-      <c r="R49" s="53"/>
-      <c r="S49" s="53"/>
-      <c r="T49" s="53"/>
-      <c r="U49" s="53"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="51"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="51"/>
+      <c r="O49" s="51"/>
+      <c r="P49" s="51"/>
+      <c r="Q49" s="51"/>
+      <c r="R49" s="51"/>
+      <c r="S49" s="51"/>
+      <c r="T49" s="51"/>
+      <c r="U49" s="51"/>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
@@ -2812,27 +2924,27 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="54"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="60"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="53"/>
-      <c r="M50" s="59"/>
-      <c r="N50" s="53"/>
-      <c r="O50" s="53"/>
-      <c r="P50" s="53"/>
-      <c r="Q50" s="53"/>
-      <c r="R50" s="53"/>
-      <c r="S50" s="53"/>
-      <c r="T50" s="53"/>
-      <c r="U50" s="53"/>
+      <c r="A50" s="52"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
+      <c r="M50" s="57"/>
+      <c r="N50" s="51"/>
+      <c r="O50" s="51"/>
+      <c r="P50" s="51"/>
+      <c r="Q50" s="51"/>
+      <c r="R50" s="51"/>
+      <c r="S50" s="51"/>
+      <c r="T50" s="51"/>
+      <c r="U50" s="51"/>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
@@ -2840,27 +2952,27 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="54"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="60"/>
-      <c r="K51" s="53"/>
-      <c r="L51" s="53"/>
-      <c r="M51" s="59"/>
-      <c r="N51" s="53"/>
-      <c r="O51" s="53"/>
-      <c r="P51" s="53"/>
-      <c r="Q51" s="53"/>
-      <c r="R51" s="53"/>
-      <c r="S51" s="53"/>
-      <c r="T51" s="53"/>
-      <c r="U51" s="53"/>
+      <c r="A51" s="52"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="58"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="57"/>
+      <c r="N51" s="51"/>
+      <c r="O51" s="51"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="51"/>
+      <c r="R51" s="51"/>
+      <c r="S51" s="51"/>
+      <c r="T51" s="51"/>
+      <c r="U51" s="51"/>
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
@@ -2868,27 +2980,27 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="54"/>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="60"/>
-      <c r="K52" s="53"/>
-      <c r="L52" s="53"/>
-      <c r="M52" s="59"/>
-      <c r="N52" s="53"/>
-      <c r="O52" s="53"/>
-      <c r="P52" s="53"/>
-      <c r="Q52" s="53"/>
-      <c r="R52" s="53"/>
-      <c r="S52" s="53"/>
-      <c r="T52" s="53"/>
-      <c r="U52" s="53"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="51"/>
+      <c r="O52" s="51"/>
+      <c r="P52" s="51"/>
+      <c r="Q52" s="51"/>
+      <c r="R52" s="51"/>
+      <c r="S52" s="51"/>
+      <c r="T52" s="51"/>
+      <c r="U52" s="51"/>
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
@@ -2896,27 +3008,27 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="54"/>
-      <c r="B53" s="55"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="55"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="60"/>
-      <c r="K53" s="53"/>
-      <c r="L53" s="53"/>
-      <c r="M53" s="59"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53"/>
-      <c r="P53" s="53"/>
-      <c r="Q53" s="53"/>
-      <c r="R53" s="53"/>
-      <c r="S53" s="53"/>
-      <c r="T53" s="53"/>
-      <c r="U53" s="53"/>
+      <c r="A53" s="52"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="58"/>
+      <c r="K53" s="51"/>
+      <c r="L53" s="51"/>
+      <c r="M53" s="57"/>
+      <c r="N53" s="51"/>
+      <c r="O53" s="51"/>
+      <c r="P53" s="51"/>
+      <c r="Q53" s="51"/>
+      <c r="R53" s="51"/>
+      <c r="S53" s="51"/>
+      <c r="T53" s="51"/>
+      <c r="U53" s="51"/>
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
@@ -2924,27 +3036,27 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="54"/>
-      <c r="B54" s="55"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="59"/>
-      <c r="J54" s="60"/>
-      <c r="K54" s="53"/>
-      <c r="L54" s="53"/>
-      <c r="M54" s="59"/>
-      <c r="N54" s="53"/>
-      <c r="O54" s="53"/>
-      <c r="P54" s="53"/>
-      <c r="Q54" s="53"/>
-      <c r="R54" s="53"/>
-      <c r="S54" s="53"/>
-      <c r="T54" s="53"/>
-      <c r="U54" s="53"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="56"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="57"/>
+      <c r="J54" s="58"/>
+      <c r="K54" s="51"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="57"/>
+      <c r="N54" s="51"/>
+      <c r="O54" s="51"/>
+      <c r="P54" s="51"/>
+      <c r="Q54" s="51"/>
+      <c r="R54" s="51"/>
+      <c r="S54" s="51"/>
+      <c r="T54" s="51"/>
+      <c r="U54" s="51"/>
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
@@ -2952,27 +3064,27 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="54"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="60"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="53"/>
-      <c r="M55" s="59"/>
-      <c r="N55" s="53"/>
-      <c r="O55" s="53"/>
-      <c r="P55" s="53"/>
-      <c r="Q55" s="53"/>
-      <c r="R55" s="53"/>
-      <c r="S55" s="53"/>
-      <c r="T55" s="53"/>
-      <c r="U55" s="53"/>
+      <c r="A55" s="52"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="57"/>
+      <c r="J55" s="58"/>
+      <c r="K55" s="51"/>
+      <c r="L55" s="51"/>
+      <c r="M55" s="57"/>
+      <c r="N55" s="51"/>
+      <c r="O55" s="51"/>
+      <c r="P55" s="51"/>
+      <c r="Q55" s="51"/>
+      <c r="R55" s="51"/>
+      <c r="S55" s="51"/>
+      <c r="T55" s="51"/>
+      <c r="U55" s="51"/>
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
@@ -2980,27 +3092,27 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="54"/>
-      <c r="B56" s="55"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="55"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="59"/>
-      <c r="J56" s="60"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="53"/>
-      <c r="M56" s="59"/>
-      <c r="N56" s="53"/>
-      <c r="O56" s="53"/>
-      <c r="P56" s="53"/>
-      <c r="Q56" s="53"/>
-      <c r="R56" s="53"/>
-      <c r="S56" s="53"/>
-      <c r="T56" s="53"/>
-      <c r="U56" s="53"/>
+      <c r="A56" s="52"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="57"/>
+      <c r="J56" s="58"/>
+      <c r="K56" s="51"/>
+      <c r="L56" s="51"/>
+      <c r="M56" s="57"/>
+      <c r="N56" s="51"/>
+      <c r="O56" s="51"/>
+      <c r="P56" s="51"/>
+      <c r="Q56" s="51"/>
+      <c r="R56" s="51"/>
+      <c r="S56" s="51"/>
+      <c r="T56" s="51"/>
+      <c r="U56" s="51"/>
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
@@ -3008,27 +3120,27 @@
       <c r="Z56" s="1"/>
     </row>
     <row r="57" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="54"/>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="56"/>
-      <c r="F57" s="61"/>
-      <c r="G57" s="61"/>
-      <c r="H57" s="61"/>
-      <c r="I57" s="59"/>
-      <c r="J57" s="60"/>
-      <c r="K57" s="53"/>
-      <c r="L57" s="53"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="53"/>
-      <c r="O57" s="53"/>
-      <c r="P57" s="53"/>
-      <c r="Q57" s="53"/>
-      <c r="R57" s="53"/>
-      <c r="S57" s="53"/>
-      <c r="T57" s="53"/>
-      <c r="U57" s="53"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="57"/>
+      <c r="J57" s="58"/>
+      <c r="K57" s="51"/>
+      <c r="L57" s="51"/>
+      <c r="M57" s="58"/>
+      <c r="N57" s="51"/>
+      <c r="O57" s="51"/>
+      <c r="P57" s="51"/>
+      <c r="Q57" s="51"/>
+      <c r="R57" s="51"/>
+      <c r="S57" s="51"/>
+      <c r="T57" s="51"/>
+      <c r="U57" s="51"/>
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
@@ -3036,27 +3148,27 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="54"/>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="64"/>
-      <c r="H58" s="64"/>
-      <c r="I58" s="59"/>
-      <c r="J58" s="60"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="53"/>
-      <c r="M58" s="60"/>
-      <c r="N58" s="53"/>
-      <c r="O58" s="53"/>
-      <c r="P58" s="53"/>
-      <c r="Q58" s="53"/>
-      <c r="R58" s="53"/>
-      <c r="S58" s="53"/>
-      <c r="T58" s="53"/>
-      <c r="U58" s="53"/>
+      <c r="A58" s="52"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="62"/>
+      <c r="G58" s="62"/>
+      <c r="H58" s="62"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="58"/>
+      <c r="K58" s="51"/>
+      <c r="L58" s="51"/>
+      <c r="M58" s="58"/>
+      <c r="N58" s="51"/>
+      <c r="O58" s="51"/>
+      <c r="P58" s="51"/>
+      <c r="Q58" s="51"/>
+      <c r="R58" s="51"/>
+      <c r="S58" s="51"/>
+      <c r="T58" s="51"/>
+      <c r="U58" s="51"/>
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
@@ -3064,27 +3176,27 @@
       <c r="Z58" s="1"/>
     </row>
     <row r="59" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="54"/>
-      <c r="B59" s="55"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="56"/>
-      <c r="E59" s="56"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="65"/>
-      <c r="I59" s="59"/>
-      <c r="J59" s="53"/>
-      <c r="K59" s="53"/>
-      <c r="L59" s="53"/>
-      <c r="M59" s="59"/>
-      <c r="N59" s="53"/>
-      <c r="O59" s="53"/>
-      <c r="P59" s="53"/>
-      <c r="Q59" s="53"/>
-      <c r="R59" s="53"/>
-      <c r="S59" s="53"/>
-      <c r="T59" s="53"/>
-      <c r="U59" s="53"/>
+      <c r="A59" s="52"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
+      <c r="L59" s="51"/>
+      <c r="M59" s="57"/>
+      <c r="N59" s="51"/>
+      <c r="O59" s="51"/>
+      <c r="P59" s="51"/>
+      <c r="Q59" s="51"/>
+      <c r="R59" s="51"/>
+      <c r="S59" s="51"/>
+      <c r="T59" s="51"/>
+      <c r="U59" s="51"/>
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
@@ -3155,7 +3267,7 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="45"/>
+      <c r="A69" s="44"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -3183,7 +3295,7 @@
       <c r="Z69" s="1"/>
     </row>
     <row r="70" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="45"/>
+      <c r="A70" s="44"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -3211,7 +3323,7 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="45"/>
+      <c r="A71" s="44"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -3239,7 +3351,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="45"/>
+      <c r="A72" s="44"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -3267,7 +3379,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="45"/>
+      <c r="A73" s="44"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -3295,7 +3407,7 @@
       <c r="Z73" s="1"/>
     </row>
     <row r="74" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="45"/>
+      <c r="A74" s="44"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -3323,7 +3435,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="45"/>
+      <c r="A75" s="44"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -3351,7 +3463,7 @@
       <c r="Z75" s="1"/>
     </row>
     <row r="76" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="45"/>
+      <c r="A76" s="44"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -3379,7 +3491,7 @@
       <c r="Z76" s="1"/>
     </row>
     <row r="77" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="45"/>
+      <c r="A77" s="44"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -3407,7 +3519,7 @@
       <c r="Z77" s="1"/>
     </row>
     <row r="78" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="45"/>
+      <c r="A78" s="44"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -3435,7 +3547,7 @@
       <c r="Z78" s="1"/>
     </row>
     <row r="79" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="45"/>
+      <c r="A79" s="44"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -3463,7 +3575,7 @@
       <c r="Z79" s="1"/>
     </row>
     <row r="80" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="45"/>
+      <c r="A80" s="44"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3491,7 +3603,7 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="45"/>
+      <c r="A81" s="44"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3519,7 +3631,7 @@
       <c r="Z81" s="1"/>
     </row>
     <row r="82" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="45"/>
+      <c r="A82" s="44"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -3547,7 +3659,7 @@
       <c r="Z82" s="1"/>
     </row>
     <row r="83" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="45"/>
+      <c r="A83" s="44"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -3575,7 +3687,7 @@
       <c r="Z83" s="1"/>
     </row>
     <row r="84" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="45"/>
+      <c r="A84" s="44"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -3603,7 +3715,7 @@
       <c r="Z84" s="1"/>
     </row>
     <row r="85" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="45"/>
+      <c r="A85" s="44"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -3631,7 +3743,7 @@
       <c r="Z85" s="1"/>
     </row>
     <row r="86" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="45"/>
+      <c r="A86" s="44"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -3659,7 +3771,7 @@
       <c r="Z86" s="1"/>
     </row>
     <row r="87" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="45"/>
+      <c r="A87" s="44"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -3687,7 +3799,7 @@
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="45"/>
+      <c r="A88" s="44"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -3715,7 +3827,7 @@
       <c r="Z88" s="1"/>
     </row>
     <row r="89" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="45"/>
+      <c r="A89" s="44"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -3743,7 +3855,7 @@
       <c r="Z89" s="1"/>
     </row>
     <row r="90" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="45"/>
+      <c r="A90" s="44"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -3771,7 +3883,7 @@
       <c r="Z90" s="1"/>
     </row>
     <row r="91" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="45"/>
+      <c r="A91" s="44"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -3799,7 +3911,7 @@
       <c r="Z91" s="1"/>
     </row>
     <row r="92" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="45"/>
+      <c r="A92" s="44"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -3827,7 +3939,7 @@
       <c r="Z92" s="1"/>
     </row>
     <row r="93" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="45"/>
+      <c r="A93" s="44"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -3855,7 +3967,7 @@
       <c r="Z93" s="1"/>
     </row>
     <row r="94" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="45"/>
+      <c r="A94" s="44"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -3883,7 +3995,7 @@
       <c r="Z94" s="1"/>
     </row>
     <row r="95" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="45"/>
+      <c r="A95" s="44"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -3911,7 +4023,7 @@
       <c r="Z95" s="1"/>
     </row>
     <row r="96" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="45"/>
+      <c r="A96" s="44"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -3939,7 +4051,7 @@
       <c r="Z96" s="1"/>
     </row>
     <row r="97" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="45"/>
+      <c r="A97" s="44"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -3967,7 +4079,7 @@
       <c r="Z97" s="1"/>
     </row>
     <row r="98" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="45"/>
+      <c r="A98" s="44"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -3995,7 +4107,7 @@
       <c r="Z98" s="1"/>
     </row>
     <row r="99" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="45"/>
+      <c r="A99" s="44"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -4023,7 +4135,7 @@
       <c r="Z99" s="1"/>
     </row>
     <row r="100" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="45"/>
+      <c r="A100" s="44"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -4051,7 +4163,7 @@
       <c r="Z100" s="1"/>
     </row>
     <row r="101" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="45"/>
+      <c r="A101" s="44"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -4079,7 +4191,7 @@
       <c r="Z101" s="1"/>
     </row>
     <row r="102" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="45"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -4107,7 +4219,7 @@
       <c r="Z102" s="1"/>
     </row>
     <row r="103" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="45"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -4135,7 +4247,7 @@
       <c r="Z103" s="1"/>
     </row>
     <row r="104" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="45"/>
+      <c r="A104" s="44"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -4163,7 +4275,7 @@
       <c r="Z104" s="1"/>
     </row>
     <row r="105" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="45"/>
+      <c r="A105" s="44"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -4191,7 +4303,7 @@
       <c r="Z105" s="1"/>
     </row>
     <row r="106" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="45"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -4219,7 +4331,7 @@
       <c r="Z106" s="1"/>
     </row>
     <row r="107" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="45"/>
+      <c r="A107" s="44"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -4247,7 +4359,7 @@
       <c r="Z107" s="1"/>
     </row>
     <row r="108" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="45"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -4275,7 +4387,7 @@
       <c r="Z108" s="1"/>
     </row>
     <row r="109" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="45"/>
+      <c r="A109" s="44"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -4303,7 +4415,7 @@
       <c r="Z109" s="1"/>
     </row>
     <row r="110" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="45"/>
+      <c r="A110" s="44"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -4331,7 +4443,7 @@
       <c r="Z110" s="1"/>
     </row>
     <row r="111" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="45"/>
+      <c r="A111" s="44"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -4359,7 +4471,7 @@
       <c r="Z111" s="1"/>
     </row>
     <row r="112" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="45"/>
+      <c r="A112" s="44"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -4387,7 +4499,7 @@
       <c r="Z112" s="1"/>
     </row>
     <row r="113" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="45"/>
+      <c r="A113" s="44"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -4415,7 +4527,7 @@
       <c r="Z113" s="1"/>
     </row>
     <row r="114" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="45"/>
+      <c r="A114" s="44"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -4443,7 +4555,7 @@
       <c r="Z114" s="1"/>
     </row>
     <row r="115" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="45"/>
+      <c r="A115" s="44"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -4471,7 +4583,7 @@
       <c r="Z115" s="1"/>
     </row>
     <row r="116" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="45"/>
+      <c r="A116" s="44"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -4499,7 +4611,7 @@
       <c r="Z116" s="1"/>
     </row>
     <row r="117" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="45"/>
+      <c r="A117" s="44"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -4527,7 +4639,7 @@
       <c r="Z117" s="1"/>
     </row>
     <row r="118" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="45"/>
+      <c r="A118" s="44"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -4555,7 +4667,7 @@
       <c r="Z118" s="1"/>
     </row>
     <row r="119" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="45"/>
+      <c r="A119" s="44"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -4583,7 +4695,7 @@
       <c r="Z119" s="1"/>
     </row>
     <row r="120" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="45"/>
+      <c r="A120" s="44"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -4611,7 +4723,7 @@
       <c r="Z120" s="1"/>
     </row>
     <row r="121" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="45"/>
+      <c r="A121" s="44"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -4639,7 +4751,7 @@
       <c r="Z121" s="1"/>
     </row>
     <row r="122" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="45"/>
+      <c r="A122" s="44"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -4667,7 +4779,7 @@
       <c r="Z122" s="1"/>
     </row>
     <row r="123" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="45"/>
+      <c r="A123" s="44"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
@@ -4695,7 +4807,7 @@
       <c r="Z123" s="1"/>
     </row>
     <row r="124" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="45"/>
+      <c r="A124" s="44"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -4723,7 +4835,7 @@
       <c r="Z124" s="1"/>
     </row>
     <row r="125" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="45"/>
+      <c r="A125" s="44"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -4751,7 +4863,7 @@
       <c r="Z125" s="1"/>
     </row>
     <row r="126" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="45"/>
+      <c r="A126" s="44"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -4779,7 +4891,7 @@
       <c r="Z126" s="1"/>
     </row>
     <row r="127" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="45"/>
+      <c r="A127" s="44"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -4807,7 +4919,7 @@
       <c r="Z127" s="1"/>
     </row>
     <row r="128" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="45"/>
+      <c r="A128" s="44"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -4835,7 +4947,7 @@
       <c r="Z128" s="1"/>
     </row>
     <row r="129" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="45"/>
+      <c r="A129" s="44"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
@@ -4863,7 +4975,7 @@
       <c r="Z129" s="1"/>
     </row>
     <row r="130" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="45"/>
+      <c r="A130" s="44"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -4891,7 +5003,7 @@
       <c r="Z130" s="1"/>
     </row>
     <row r="131" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="45"/>
+      <c r="A131" s="44"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -4919,7 +5031,7 @@
       <c r="Z131" s="1"/>
     </row>
     <row r="132" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="45"/>
+      <c r="A132" s="44"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
@@ -4947,7 +5059,7 @@
       <c r="Z132" s="1"/>
     </row>
     <row r="133" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="45"/>
+      <c r="A133" s="44"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -4975,7 +5087,7 @@
       <c r="Z133" s="1"/>
     </row>
     <row r="134" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="45"/>
+      <c r="A134" s="44"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -5003,7 +5115,7 @@
       <c r="Z134" s="1"/>
     </row>
     <row r="135" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="45"/>
+      <c r="A135" s="44"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -5031,7 +5143,7 @@
       <c r="Z135" s="1"/>
     </row>
     <row r="136" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="45"/>
+      <c r="A136" s="44"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -5059,7 +5171,7 @@
       <c r="Z136" s="1"/>
     </row>
     <row r="137" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="45"/>
+      <c r="A137" s="44"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -5087,7 +5199,7 @@
       <c r="Z137" s="1"/>
     </row>
     <row r="138" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="45"/>
+      <c r="A138" s="44"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -5115,7 +5227,7 @@
       <c r="Z138" s="1"/>
     </row>
     <row r="139" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="45"/>
+      <c r="A139" s="44"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -5143,7 +5255,7 @@
       <c r="Z139" s="1"/>
     </row>
     <row r="140" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="45"/>
+      <c r="A140" s="44"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -5171,7 +5283,7 @@
       <c r="Z140" s="1"/>
     </row>
     <row r="141" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="45"/>
+      <c r="A141" s="44"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
@@ -5199,7 +5311,7 @@
       <c r="Z141" s="1"/>
     </row>
     <row r="142" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="45"/>
+      <c r="A142" s="44"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -5227,7 +5339,7 @@
       <c r="Z142" s="1"/>
     </row>
     <row r="143" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="45"/>
+      <c r="A143" s="44"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -5255,7 +5367,7 @@
       <c r="Z143" s="1"/>
     </row>
     <row r="144" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="45"/>
+      <c r="A144" s="44"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -5283,7 +5395,7 @@
       <c r="Z144" s="1"/>
     </row>
     <row r="145" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="45"/>
+      <c r="A145" s="44"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
@@ -5311,7 +5423,7 @@
       <c r="Z145" s="1"/>
     </row>
     <row r="146" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="45"/>
+      <c r="A146" s="44"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
@@ -5339,7 +5451,7 @@
       <c r="Z146" s="1"/>
     </row>
     <row r="147" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="45"/>
+      <c r="A147" s="44"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
@@ -5367,7 +5479,7 @@
       <c r="Z147" s="1"/>
     </row>
     <row r="148" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="45"/>
+      <c r="A148" s="44"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
@@ -5395,7 +5507,7 @@
       <c r="Z148" s="1"/>
     </row>
     <row r="149" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="45"/>
+      <c r="A149" s="44"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
@@ -5423,7 +5535,7 @@
       <c r="Z149" s="1"/>
     </row>
     <row r="150" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="45"/>
+      <c r="A150" s="44"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
@@ -5451,7 +5563,7 @@
       <c r="Z150" s="1"/>
     </row>
     <row r="151" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="45"/>
+      <c r="A151" s="44"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
@@ -5479,7 +5591,7 @@
       <c r="Z151" s="1"/>
     </row>
     <row r="152" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="45"/>
+      <c r="A152" s="44"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -5507,7 +5619,7 @@
       <c r="Z152" s="1"/>
     </row>
     <row r="153" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="45"/>
+      <c r="A153" s="44"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -5535,7 +5647,7 @@
       <c r="Z153" s="1"/>
     </row>
     <row r="154" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="45"/>
+      <c r="A154" s="44"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -5563,7 +5675,7 @@
       <c r="Z154" s="1"/>
     </row>
     <row r="155" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="45"/>
+      <c r="A155" s="44"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
@@ -5591,7 +5703,7 @@
       <c r="Z155" s="1"/>
     </row>
     <row r="156" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="45"/>
+      <c r="A156" s="44"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
@@ -5619,7 +5731,7 @@
       <c r="Z156" s="1"/>
     </row>
     <row r="157" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="45"/>
+      <c r="A157" s="44"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
@@ -5647,7 +5759,7 @@
       <c r="Z157" s="1"/>
     </row>
     <row r="158" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="45"/>
+      <c r="A158" s="44"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
@@ -5675,7 +5787,7 @@
       <c r="Z158" s="1"/>
     </row>
     <row r="159" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="45"/>
+      <c r="A159" s="44"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
@@ -5703,7 +5815,7 @@
       <c r="Z159" s="1"/>
     </row>
     <row r="160" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="45"/>
+      <c r="A160" s="44"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
@@ -5731,7 +5843,7 @@
       <c r="Z160" s="1"/>
     </row>
     <row r="161" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="45"/>
+      <c r="A161" s="44"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
@@ -5759,7 +5871,7 @@
       <c r="Z161" s="1"/>
     </row>
     <row r="162" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="45"/>
+      <c r="A162" s="44"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -5787,7 +5899,7 @@
       <c r="Z162" s="1"/>
     </row>
     <row r="163" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="45"/>
+      <c r="A163" s="44"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -5815,7 +5927,7 @@
       <c r="Z163" s="1"/>
     </row>
     <row r="164" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="45"/>
+      <c r="A164" s="44"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
@@ -5843,7 +5955,7 @@
       <c r="Z164" s="1"/>
     </row>
     <row r="165" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="45"/>
+      <c r="A165" s="44"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
@@ -5871,7 +5983,7 @@
       <c r="Z165" s="1"/>
     </row>
     <row r="166" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="45"/>
+      <c r="A166" s="44"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
@@ -5899,7 +6011,7 @@
       <c r="Z166" s="1"/>
     </row>
     <row r="167" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="45"/>
+      <c r="A167" s="44"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -5927,7 +6039,7 @@
       <c r="Z167" s="1"/>
     </row>
     <row r="168" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="45"/>
+      <c r="A168" s="44"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
@@ -5955,7 +6067,7 @@
       <c r="Z168" s="1"/>
     </row>
     <row r="169" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="45"/>
+      <c r="A169" s="44"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -5983,7 +6095,7 @@
       <c r="Z169" s="1"/>
     </row>
     <row r="170" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="45"/>
+      <c r="A170" s="44"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
@@ -6011,7 +6123,7 @@
       <c r="Z170" s="1"/>
     </row>
     <row r="171" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="45"/>
+      <c r="A171" s="44"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
@@ -6039,7 +6151,7 @@
       <c r="Z171" s="1"/>
     </row>
     <row r="172" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="45"/>
+      <c r="A172" s="44"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
@@ -6067,7 +6179,7 @@
       <c r="Z172" s="1"/>
     </row>
     <row r="173" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="45"/>
+      <c r="A173" s="44"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
@@ -6095,7 +6207,7 @@
       <c r="Z173" s="1"/>
     </row>
     <row r="174" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="45"/>
+      <c r="A174" s="44"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
@@ -6123,7 +6235,7 @@
       <c r="Z174" s="1"/>
     </row>
     <row r="175" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="45"/>
+      <c r="A175" s="44"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
@@ -6151,7 +6263,7 @@
       <c r="Z175" s="1"/>
     </row>
     <row r="176" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="45"/>
+      <c r="A176" s="44"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
@@ -6179,7 +6291,7 @@
       <c r="Z176" s="1"/>
     </row>
     <row r="177" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="45"/>
+      <c r="A177" s="44"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -6207,7 +6319,7 @@
       <c r="Z177" s="1"/>
     </row>
     <row r="178" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="45"/>
+      <c r="A178" s="44"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -6235,7 +6347,7 @@
       <c r="Z178" s="1"/>
     </row>
     <row r="179" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="45"/>
+      <c r="A179" s="44"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -6263,7 +6375,7 @@
       <c r="Z179" s="1"/>
     </row>
     <row r="180" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="45"/>
+      <c r="A180" s="44"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
@@ -6291,7 +6403,7 @@
       <c r="Z180" s="1"/>
     </row>
     <row r="181" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="45"/>
+      <c r="A181" s="44"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
@@ -6319,7 +6431,7 @@
       <c r="Z181" s="1"/>
     </row>
     <row r="182" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="45"/>
+      <c r="A182" s="44"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
@@ -6347,7 +6459,7 @@
       <c r="Z182" s="1"/>
     </row>
     <row r="183" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="45"/>
+      <c r="A183" s="44"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
@@ -6375,7 +6487,7 @@
       <c r="Z183" s="1"/>
     </row>
     <row r="184" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="45"/>
+      <c r="A184" s="44"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
@@ -6403,7 +6515,7 @@
       <c r="Z184" s="1"/>
     </row>
     <row r="185" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="45"/>
+      <c r="A185" s="44"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
@@ -6431,7 +6543,7 @@
       <c r="Z185" s="1"/>
     </row>
     <row r="186" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="45"/>
+      <c r="A186" s="44"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
@@ -6459,7 +6571,7 @@
       <c r="Z186" s="1"/>
     </row>
     <row r="187" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="45"/>
+      <c r="A187" s="44"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
@@ -6487,7 +6599,7 @@
       <c r="Z187" s="1"/>
     </row>
     <row r="188" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="45"/>
+      <c r="A188" s="44"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
@@ -6515,7 +6627,7 @@
       <c r="Z188" s="1"/>
     </row>
     <row r="189" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="45"/>
+      <c r="A189" s="44"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
@@ -6543,7 +6655,7 @@
       <c r="Z189" s="1"/>
     </row>
     <row r="190" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="45"/>
+      <c r="A190" s="44"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
@@ -6571,7 +6683,7 @@
       <c r="Z190" s="1"/>
     </row>
     <row r="191" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="45"/>
+      <c r="A191" s="44"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
@@ -6599,7 +6711,7 @@
       <c r="Z191" s="1"/>
     </row>
     <row r="192" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="45"/>
+      <c r="A192" s="44"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
@@ -6627,7 +6739,7 @@
       <c r="Z192" s="1"/>
     </row>
     <row r="193" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="45"/>
+      <c r="A193" s="44"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
@@ -6655,7 +6767,7 @@
       <c r="Z193" s="1"/>
     </row>
     <row r="194" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="45"/>
+      <c r="A194" s="44"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
@@ -6683,7 +6795,7 @@
       <c r="Z194" s="1"/>
     </row>
     <row r="195" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="45"/>
+      <c r="A195" s="44"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
@@ -6711,7 +6823,7 @@
       <c r="Z195" s="1"/>
     </row>
     <row r="196" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="45"/>
+      <c r="A196" s="44"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
@@ -6739,7 +6851,7 @@
       <c r="Z196" s="1"/>
     </row>
     <row r="197" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="45"/>
+      <c r="A197" s="44"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -6767,7 +6879,7 @@
       <c r="Z197" s="1"/>
     </row>
     <row r="198" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="45"/>
+      <c r="A198" s="44"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
@@ -6795,7 +6907,7 @@
       <c r="Z198" s="1"/>
     </row>
     <row r="199" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="45"/>
+      <c r="A199" s="44"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
@@ -6823,7 +6935,7 @@
       <c r="Z199" s="1"/>
     </row>
     <row r="200" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="45"/>
+      <c r="A200" s="44"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
@@ -6851,7 +6963,7 @@
       <c r="Z200" s="1"/>
     </row>
     <row r="201" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="45"/>
+      <c r="A201" s="44"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -6879,7 +6991,7 @@
       <c r="Z201" s="1"/>
     </row>
     <row r="202" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="45"/>
+      <c r="A202" s="44"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
@@ -6907,7 +7019,7 @@
       <c r="Z202" s="1"/>
     </row>
     <row r="203" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="45"/>
+      <c r="A203" s="44"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
@@ -6935,7 +7047,7 @@
       <c r="Z203" s="1"/>
     </row>
     <row r="204" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="45"/>
+      <c r="A204" s="44"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
@@ -6963,7 +7075,7 @@
       <c r="Z204" s="1"/>
     </row>
     <row r="205" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="45"/>
+      <c r="A205" s="44"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
@@ -6991,7 +7103,7 @@
       <c r="Z205" s="1"/>
     </row>
     <row r="206" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="45"/>
+      <c r="A206" s="44"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
@@ -7019,7 +7131,7 @@
       <c r="Z206" s="1"/>
     </row>
     <row r="207" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="45"/>
+      <c r="A207" s="44"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
@@ -7047,7 +7159,7 @@
       <c r="Z207" s="1"/>
     </row>
     <row r="208" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="45"/>
+      <c r="A208" s="44"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
@@ -7075,7 +7187,7 @@
       <c r="Z208" s="1"/>
     </row>
     <row r="209" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="45"/>
+      <c r="A209" s="44"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
@@ -7103,7 +7215,7 @@
       <c r="Z209" s="1"/>
     </row>
     <row r="210" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="45"/>
+      <c r="A210" s="44"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
@@ -7131,7 +7243,7 @@
       <c r="Z210" s="1"/>
     </row>
     <row r="211" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="45"/>
+      <c r="A211" s="44"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
@@ -7159,7 +7271,7 @@
       <c r="Z211" s="1"/>
     </row>
     <row r="212" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="45"/>
+      <c r="A212" s="44"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
@@ -7187,7 +7299,7 @@
       <c r="Z212" s="1"/>
     </row>
     <row r="213" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="45"/>
+      <c r="A213" s="44"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
@@ -7215,7 +7327,7 @@
       <c r="Z213" s="1"/>
     </row>
     <row r="214" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="45"/>
+      <c r="A214" s="44"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
@@ -7243,7 +7355,7 @@
       <c r="Z214" s="1"/>
     </row>
     <row r="215" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="45"/>
+      <c r="A215" s="44"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
@@ -7271,7 +7383,7 @@
       <c r="Z215" s="1"/>
     </row>
     <row r="216" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="45"/>
+      <c r="A216" s="44"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
@@ -7299,7 +7411,7 @@
       <c r="Z216" s="1"/>
     </row>
     <row r="217" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="45"/>
+      <c r="A217" s="44"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
@@ -7327,7 +7439,7 @@
       <c r="Z217" s="1"/>
     </row>
     <row r="218" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="45"/>
+      <c r="A218" s="44"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -7355,7 +7467,7 @@
       <c r="Z218" s="1"/>
     </row>
     <row r="219" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="45"/>
+      <c r="A219" s="44"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
@@ -7383,7 +7495,7 @@
       <c r="Z219" s="1"/>
     </row>
     <row r="220" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="45"/>
+      <c r="A220" s="44"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
@@ -7411,7 +7523,7 @@
       <c r="Z220" s="1"/>
     </row>
     <row r="221" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="45"/>
+      <c r="A221" s="44"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
@@ -7439,7 +7551,7 @@
       <c r="Z221" s="1"/>
     </row>
     <row r="222" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="45"/>
+      <c r="A222" s="44"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
@@ -7467,7 +7579,7 @@
       <c r="Z222" s="1"/>
     </row>
     <row r="223" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="45"/>
+      <c r="A223" s="44"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
@@ -7495,7 +7607,7 @@
       <c r="Z223" s="1"/>
     </row>
     <row r="224" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="45"/>
+      <c r="A224" s="44"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
@@ -7523,7 +7635,7 @@
       <c r="Z224" s="1"/>
     </row>
     <row r="225" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="45"/>
+      <c r="A225" s="44"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
@@ -7551,7 +7663,7 @@
       <c r="Z225" s="1"/>
     </row>
     <row r="226" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="45"/>
+      <c r="A226" s="44"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
@@ -7579,7 +7691,7 @@
       <c r="Z226" s="1"/>
     </row>
     <row r="227" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="45"/>
+      <c r="A227" s="44"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
@@ -7607,7 +7719,7 @@
       <c r="Z227" s="1"/>
     </row>
     <row r="228" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="45"/>
+      <c r="A228" s="44"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
@@ -7635,7 +7747,7 @@
       <c r="Z228" s="1"/>
     </row>
     <row r="229" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="45"/>
+      <c r="A229" s="44"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
@@ -7663,7 +7775,7 @@
       <c r="Z229" s="1"/>
     </row>
     <row r="230" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="45"/>
+      <c r="A230" s="44"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
@@ -7691,7 +7803,7 @@
       <c r="Z230" s="1"/>
     </row>
     <row r="231" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="45"/>
+      <c r="A231" s="44"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>
@@ -7719,7 +7831,7 @@
       <c r="Z231" s="1"/>
     </row>
     <row r="232" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="45"/>
+      <c r="A232" s="44"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
       <c r="D232" s="1"/>
@@ -7747,7 +7859,7 @@
       <c r="Z232" s="1"/>
     </row>
     <row r="233" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="45"/>
+      <c r="A233" s="44"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
       <c r="D233" s="1"/>
@@ -7775,7 +7887,7 @@
       <c r="Z233" s="1"/>
     </row>
     <row r="234" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="45"/>
+      <c r="A234" s="44"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
@@ -7803,7 +7915,7 @@
       <c r="Z234" s="1"/>
     </row>
     <row r="235" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="45"/>
+      <c r="A235" s="44"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
@@ -7831,7 +7943,7 @@
       <c r="Z235" s="1"/>
     </row>
     <row r="236" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="45"/>
+      <c r="A236" s="44"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
@@ -7859,7 +7971,7 @@
       <c r="Z236" s="1"/>
     </row>
     <row r="237" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="45"/>
+      <c r="A237" s="44"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
@@ -7887,7 +7999,7 @@
       <c r="Z237" s="1"/>
     </row>
     <row r="238" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="45"/>
+      <c r="A238" s="44"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
@@ -7915,7 +8027,7 @@
       <c r="Z238" s="1"/>
     </row>
     <row r="239" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="45"/>
+      <c r="A239" s="44"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
@@ -7943,7 +8055,7 @@
       <c r="Z239" s="1"/>
     </row>
     <row r="240" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="45"/>
+      <c r="A240" s="44"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
@@ -7971,7 +8083,7 @@
       <c r="Z240" s="1"/>
     </row>
     <row r="241" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="45"/>
+      <c r="A241" s="44"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -7999,7 +8111,7 @@
       <c r="Z241" s="1"/>
     </row>
     <row r="242" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="45"/>
+      <c r="A242" s="44"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -8027,7 +8139,7 @@
       <c r="Z242" s="1"/>
     </row>
     <row r="243" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="45"/>
+      <c r="A243" s="44"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
@@ -8055,7 +8167,7 @@
       <c r="Z243" s="1"/>
     </row>
     <row r="244" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="45"/>
+      <c r="A244" s="44"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
       <c r="D244" s="1"/>
@@ -8083,7 +8195,7 @@
       <c r="Z244" s="1"/>
     </row>
     <row r="245" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="45"/>
+      <c r="A245" s="44"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
       <c r="D245" s="1"/>
@@ -8111,7 +8223,7 @@
       <c r="Z245" s="1"/>
     </row>
     <row r="246" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="45"/>
+      <c r="A246" s="44"/>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
       <c r="D246" s="1"/>
@@ -8139,7 +8251,7 @@
       <c r="Z246" s="1"/>
     </row>
     <row r="247" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="45"/>
+      <c r="A247" s="44"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
@@ -8167,7 +8279,7 @@
       <c r="Z247" s="1"/>
     </row>
     <row r="248" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="45"/>
+      <c r="A248" s="44"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
@@ -8195,7 +8307,7 @@
       <c r="Z248" s="1"/>
     </row>
     <row r="249" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="45"/>
+      <c r="A249" s="44"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1"/>
@@ -8223,7 +8335,7 @@
       <c r="Z249" s="1"/>
     </row>
     <row r="250" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="45"/>
+      <c r="A250" s="44"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1"/>
@@ -8251,7 +8363,7 @@
       <c r="Z250" s="1"/>
     </row>
     <row r="251" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="45"/>
+      <c r="A251" s="44"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1"/>
@@ -8279,7 +8391,7 @@
       <c r="Z251" s="1"/>
     </row>
     <row r="252" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="45"/>
+      <c r="A252" s="44"/>
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
       <c r="D252" s="1"/>
@@ -8307,7 +8419,7 @@
       <c r="Z252" s="1"/>
     </row>
     <row r="253" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="45"/>
+      <c r="A253" s="44"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
       <c r="D253" s="1"/>
@@ -8335,7 +8447,7 @@
       <c r="Z253" s="1"/>
     </row>
     <row r="254" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="45"/>
+      <c r="A254" s="44"/>
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
       <c r="D254" s="1"/>
@@ -8363,7 +8475,7 @@
       <c r="Z254" s="1"/>
     </row>
     <row r="255" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="45"/>
+      <c r="A255" s="44"/>
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
       <c r="D255" s="1"/>
@@ -8391,7 +8503,7 @@
       <c r="Z255" s="1"/>
     </row>
     <row r="256" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="45"/>
+      <c r="A256" s="44"/>
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
       <c r="D256" s="1"/>
@@ -8419,7 +8531,7 @@
       <c r="Z256" s="1"/>
     </row>
     <row r="257" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="45"/>
+      <c r="A257" s="44"/>
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
       <c r="D257" s="1"/>
@@ -8447,7 +8559,7 @@
       <c r="Z257" s="1"/>
     </row>
     <row r="258" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="45"/>
+      <c r="A258" s="44"/>
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
       <c r="D258" s="1"/>
@@ -8475,7 +8587,7 @@
       <c r="Z258" s="1"/>
     </row>
     <row r="259" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="45"/>
+      <c r="A259" s="44"/>
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
       <c r="D259" s="1"/>
@@ -8503,7 +8615,7 @@
       <c r="Z259" s="1"/>
     </row>
     <row r="260" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="45"/>
+      <c r="A260" s="44"/>
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
       <c r="D260" s="1"/>
@@ -8531,7 +8643,7 @@
       <c r="Z260" s="1"/>
     </row>
     <row r="261" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="45"/>
+      <c r="A261" s="44"/>
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
       <c r="D261" s="1"/>
@@ -8559,7 +8671,7 @@
       <c r="Z261" s="1"/>
     </row>
     <row r="262" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="45"/>
+      <c r="A262" s="44"/>
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1"/>
@@ -8587,7 +8699,7 @@
       <c r="Z262" s="1"/>
     </row>
     <row r="263" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="45"/>
+      <c r="A263" s="44"/>
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
       <c r="D263" s="1"/>
@@ -8615,7 +8727,7 @@
       <c r="Z263" s="1"/>
     </row>
     <row r="264" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="45"/>
+      <c r="A264" s="44"/>
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
       <c r="D264" s="1"/>
@@ -8643,7 +8755,7 @@
       <c r="Z264" s="1"/>
     </row>
     <row r="265" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="45"/>
+      <c r="A265" s="44"/>
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
       <c r="D265" s="1"/>
@@ -8671,7 +8783,7 @@
       <c r="Z265" s="1"/>
     </row>
     <row r="266" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="45"/>
+      <c r="A266" s="44"/>
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
       <c r="D266" s="1"/>
@@ -8699,7 +8811,7 @@
       <c r="Z266" s="1"/>
     </row>
     <row r="267" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="45"/>
+      <c r="A267" s="44"/>
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
       <c r="D267" s="1"/>
@@ -8727,7 +8839,7 @@
       <c r="Z267" s="1"/>
     </row>
     <row r="268" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="45"/>
+      <c r="A268" s="44"/>
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
       <c r="D268" s="1"/>
@@ -9487,7 +9599,17 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="I11:L12"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
     <mergeCell ref="M11:Q12"/>
     <mergeCell ref="T12:U12"/>
     <mergeCell ref="R12:S12"/>
@@ -9499,13 +9621,6 @@
     <mergeCell ref="T15:U15"/>
     <mergeCell ref="I15:L15"/>
     <mergeCell ref="B11:E12"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="F3:L3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="I11:L12"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.27569444444444402" right="0.27569444444444402" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
feat: adjust style export excel IPa
</commit_message>
<xml_diff>
--- a/public/assets/file/Template IPA.xlsx
+++ b/public/assets/file/Template IPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87DABC7-3414-4A66-9B72-8F8802DBCFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C6F41-E371-4855-B27D-EE6CEB486097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,21 +43,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>No. Form</t>
-  </si>
-  <si>
-    <t>:  F/SOP/CHR/005-01</t>
   </si>
   <si>
     <t>PERFORMANCE APPRAISAL</t>
   </si>
   <si>
     <t>Hal</t>
-  </si>
-  <si>
-    <t>:  1 dari 3</t>
   </si>
   <si>
     <t>(One Year Result Review)</t>
@@ -136,6 +130,18 @@
   </si>
   <si>
     <t>(W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">: </t>
+  </si>
+  <si>
+    <t>1 dari 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:  </t>
+  </si>
+  <si>
+    <t>F/SOP/CHR/005-01</t>
   </si>
 </sst>
 </file>
@@ -327,7 +333,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -901,15 +907,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -922,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -994,12 +991,6 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1064,7 +1055,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1116,6 +1107,71 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1144,130 +1200,64 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1528,30 +1518,32 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.453125" style="13" customWidth="1"/>
     <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="3" max="3" width="2.81640625" customWidth="1"/>
+    <col min="4" max="4" width="33.7265625" customWidth="1"/>
     <col min="5" max="5" width="40.36328125" customWidth="1"/>
     <col min="6" max="8" width="6.08984375" customWidth="1"/>
     <col min="9" max="9" width="16.26953125" customWidth="1"/>
     <col min="10" max="10" width="12.90625" customWidth="1"/>
     <col min="11" max="11" width="21.08984375" customWidth="1"/>
     <col min="12" max="12" width="22.90625" customWidth="1"/>
-    <col min="13" max="13" width="9.7265625" customWidth="1"/>
-    <col min="14" max="16" width="9.08984375" customWidth="1"/>
-    <col min="17" max="17" width="27.08984375" customWidth="1"/>
-    <col min="18" max="20" width="5.7265625" customWidth="1"/>
-    <col min="21" max="21" width="6.6328125" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" customWidth="1"/>
+    <col min="15" max="16" width="1.81640625" customWidth="1"/>
+    <col min="17" max="17" width="13.81640625" customWidth="1"/>
+    <col min="18" max="18" width="2.81640625" customWidth="1"/>
+    <col min="19" max="20" width="5.7265625" customWidth="1"/>
+    <col min="21" max="21" width="19.1796875" customWidth="1"/>
     <col min="22" max="26" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1567,91 +1559,95 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="128" t="s">
+      <c r="P1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124" t="s">
-        <v>1</v>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82" t="s">
+        <v>31</v>
       </c>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="125"/>
+      <c r="S1" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="82"/>
+      <c r="U1" s="83"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="76" t="s">
-        <v>2</v>
+      <c r="F2" s="103" t="s">
+        <v>1</v>
       </c>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="129" t="s">
-        <v>3</v>
+      <c r="P2" s="87" t="s">
+        <v>2</v>
       </c>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110" t="s">
-        <v>4</v>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73" t="s">
+        <v>29</v>
       </c>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="130"/>
+      <c r="S2" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="73"/>
+      <c r="U2" s="88"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="78" t="s">
-        <v>5</v>
+      <c r="F3" s="105" t="s">
+        <v>3</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="129" t="s">
-        <v>6</v>
+      <c r="P3" s="87" t="s">
+        <v>4</v>
       </c>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110" t="s">
-        <v>7</v>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73" t="s">
+        <v>5</v>
       </c>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="131"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="89"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1667,23 +1663,23 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="132" t="s">
-        <v>8</v>
+      <c r="P4" s="90" t="s">
+        <v>6</v>
       </c>
-      <c r="Q4" s="126"/>
-      <c r="R4" s="126" t="s">
-        <v>7</v>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84" t="s">
+        <v>5</v>
       </c>
-      <c r="S4" s="126"/>
-      <c r="T4" s="126"/>
-      <c r="U4" s="127"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="85"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1711,115 +1707,115 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="105"/>
-      <c r="C6" s="106" t="s">
+    <row r="6" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
-      <c r="M6" s="109"/>
-      <c r="N6" s="110"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="111" t="s">
-        <v>10</v>
+      <c r="B6" s="68"/>
+      <c r="C6" s="69" t="s">
+        <v>5</v>
       </c>
-      <c r="Q6" s="107"/>
-      <c r="R6" s="106" t="s">
-        <v>7</v>
+      <c r="D6" s="69"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="74" t="s">
+        <v>8</v>
       </c>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="112"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="93"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
-        <v>11</v>
+    <row r="7" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="116" t="s">
+        <v>9</v>
       </c>
-      <c r="B7" s="114"/>
-      <c r="C7" s="115" t="s">
-        <v>7</v>
+      <c r="B7" s="117"/>
+      <c r="C7" s="75" t="s">
+        <v>5</v>
       </c>
-      <c r="D7" s="109"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="109"/>
-      <c r="J7" s="109"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="109"/>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="116" t="s">
-        <v>12</v>
+      <c r="D7" s="75"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="76" t="s">
+        <v>10</v>
       </c>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="115" t="s">
-        <v>7</v>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="75" t="s">
+        <v>5</v>
       </c>
-      <c r="S7" s="109"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="117"/>
+      <c r="S7" s="75"/>
+      <c r="T7" s="75"/>
+      <c r="U7" s="94"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
-        <v>13</v>
+    <row r="8" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="77" t="s">
+        <v>11</v>
       </c>
-      <c r="B8" s="119"/>
-      <c r="C8" s="120" t="s">
-        <v>7</v>
+      <c r="B8" s="78"/>
+      <c r="C8" s="79" t="s">
+        <v>5</v>
       </c>
-      <c r="D8" s="121"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="109"/>
-      <c r="J8" s="109"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="109"/>
-      <c r="M8" s="109"/>
-      <c r="N8" s="110"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="122" t="s">
-        <v>14</v>
+      <c r="D8" s="79"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="81" t="s">
+        <v>12</v>
       </c>
-      <c r="Q8" s="121"/>
-      <c r="R8" s="120" t="s">
-        <v>7</v>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="79" t="s">
+        <v>5</v>
       </c>
-      <c r="S8" s="121"/>
-      <c r="T8" s="121"/>
-      <c r="U8" s="123"/>
+      <c r="S8" s="79"/>
+      <c r="T8" s="79"/>
+      <c r="U8" s="95"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1847,7 +1843,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="5"/>
       <c r="C10" s="1"/>
@@ -1869,7 +1865,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="1"/>
       <c r="U10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
@@ -1877,76 +1873,76 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="88" t="s">
+    <row r="11" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="118" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="89" t="s">
+      <c r="G11" s="120"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="89" t="s">
+      <c r="J11" s="107"/>
+      <c r="K11" s="107"/>
+      <c r="L11" s="108"/>
+      <c r="M11" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="92"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="89" t="s">
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="108"/>
+      <c r="R11" s="106" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="89" t="s">
+      <c r="S11" s="115"/>
+      <c r="T11" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="90"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="91"/>
-      <c r="R11" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="S11" s="93"/>
-      <c r="T11" s="94" t="s">
-        <v>22</v>
-      </c>
-      <c r="U11" s="95"/>
+      <c r="U11" s="131"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="96"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="101"/>
-      <c r="H12" s="102"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="98"/>
-      <c r="O12" s="98"/>
-      <c r="P12" s="98"/>
-      <c r="Q12" s="99"/>
-      <c r="R12" s="100" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12" s="102"/>
-      <c r="T12" s="100" t="s">
+    <row r="12" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="119"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="U12" s="103"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="110"/>
+      <c r="K12" s="110"/>
+      <c r="L12" s="111"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="110"/>
+      <c r="O12" s="110"/>
+      <c r="P12" s="110"/>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12" s="114"/>
+      <c r="T12" s="112" t="s">
+        <v>26</v>
+      </c>
+      <c r="U12" s="113"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -1954,27 +1950,27 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="56"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="26"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="53"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="67"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="53"/>
+      <c r="U13" s="65"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -1982,68 +1978,68 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="65"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="62"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="62"/>
-      <c r="U14" s="68"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="60"/>
+      <c r="U14" s="66"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="79" t="s">
-        <v>23</v>
+    <row r="15" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="29"/>
+      <c r="B15" s="122" t="s">
+        <v>21</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="82">
+      <c r="C15" s="123"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="125">
         <f ca="1">SUM(F13:H59)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="80"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84" t="s">
-        <v>24</v>
+      <c r="G15" s="123"/>
+      <c r="H15" s="126"/>
+      <c r="I15" s="129"/>
+      <c r="J15" s="123"/>
+      <c r="K15" s="123"/>
+      <c r="L15" s="126"/>
+      <c r="M15" s="127" t="s">
+        <v>22</v>
       </c>
-      <c r="N15" s="80"/>
-      <c r="O15" s="80"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="85">
+      <c r="N15" s="123"/>
+      <c r="O15" s="123"/>
+      <c r="P15" s="123"/>
+      <c r="Q15" s="124"/>
+      <c r="R15" s="128">
         <f ca="1">SUM(R13:S59)</f>
         <v>0</v>
       </c>
-      <c r="S15" s="83"/>
-      <c r="T15" s="86">
+      <c r="S15" s="126"/>
+      <c r="T15" s="129">
         <f ca="1">SUM(T13:U59)</f>
         <v>0</v>
       </c>
-      <c r="U15" s="87"/>
+      <c r="U15" s="130"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -2051,33 +2047,33 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="69" t="s">
-        <v>25</v>
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="96" t="s">
+        <v>23</v>
       </c>
-      <c r="J16" s="70"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="72" t="s">
-        <v>14</v>
+      <c r="J16" s="97"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="99" t="s">
+        <v>12</v>
       </c>
-      <c r="M16" s="73"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="69" t="s">
-        <v>26</v>
+      <c r="M16" s="100"/>
+      <c r="N16" s="100"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="101"/>
+      <c r="Q16" s="96" t="s">
+        <v>24</v>
       </c>
-      <c r="R16" s="70"/>
-      <c r="S16" s="70"/>
-      <c r="T16" s="70"/>
-      <c r="U16" s="71"/>
+      <c r="R16" s="97"/>
+      <c r="S16" s="97"/>
+      <c r="T16" s="97"/>
+      <c r="U16" s="98"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -2085,27 +2081,27 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="39"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
+      <c r="U17" s="37"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -2113,27 +2109,27 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="29"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="30"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="28"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
@@ -2141,27 +2137,27 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="30"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="28"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
@@ -2169,27 +2165,27 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="30"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="28"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
@@ -2197,27 +2193,10 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="30"/>
+      <c r="I21" s="91"/>
+      <c r="L21" s="91"/>
+      <c r="Q21" s="91"/>
+      <c r="U21" s="92"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
@@ -2225,61 +2204,21 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="43"/>
-      <c r="T22" s="43"/>
-      <c r="U22" s="46"/>
+      <c r="I22" s="91"/>
+      <c r="L22" s="91"/>
+      <c r="Q22" s="91"/>
+      <c r="U22" s="92"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="47"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="M23" s="51"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="R23" s="48"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="52"/>
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="91"/>
+      <c r="L23" s="91"/>
+      <c r="Q23" s="91"/>
+      <c r="U23" s="92"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
@@ -2287,27 +2226,10 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
+      <c r="I24" s="91"/>
+      <c r="L24" s="91"/>
+      <c r="Q24" s="91"/>
+      <c r="U24" s="92"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -2315,27 +2237,10 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
+      <c r="I25" s="91"/>
+      <c r="L25" s="91"/>
+      <c r="Q25" s="91"/>
+      <c r="U25" s="92"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -2343,83 +2248,89 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="28"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
+    <row r="27" spans="1:26" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="44"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
+    <row r="28" spans="1:26" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="45"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="49"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="50"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
@@ -9690,7 +9601,7 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="M15:Q15"/>
@@ -9712,6 +9623,7 @@
     <mergeCell ref="T12:U12"/>
     <mergeCell ref="R12:S12"/>
     <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:U11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.27569444444444402" right="0.27569444444444402" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>